<commit_message>
19-04-21: Design Complete. First Order Placed and Payed for
</commit_message>
<xml_diff>
--- a/CommunicationBoard/Project Outputs for CommunicationBoard/BOM/Final 3 - Bill of Materials-CommunicationBoard.xlsx
+++ b/CommunicationBoard/Project Outputs for CommunicationBoard/BOM/Final 3 - Bill of Materials-CommunicationBoard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Projects\IoTAdvanced-Mesh-Gateway\CommunicationBoard\Project Outputs for CommunicationBoard\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Projects\IoTAdvanced-Mesh+Gateway\CommunicationBoard\Project Outputs for CommunicationBoard\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91AF8C7D-7DE4-4BA3-B6E8-F0C070789B57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661371D0-1181-4B5C-A610-610C5252F74B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4CE27D47-B495-4376-87C2-F434AAD08B68}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{4CE27D47-B495-4376-87C2-F434AAD08B68}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Communication" sheetId="1" r:id="rId1"/>
@@ -905,7 +905,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,7 +917,7 @@
     <col min="6" max="9" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>104</v>
       </c>

</xml_diff>